<commit_message>
test data file added
</commit_message>
<xml_diff>
--- a/files/TestData.xlsx
+++ b/files/TestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pulse.tester\eclipse-workspace\pulseSolutions_au_contactUs\files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A8D1A0-5305-4F4A-A230-A38148B6D554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -59,12 +53,15 @@
   </si>
   <si>
     <t>DRftgyhu@14</t>
+  </si>
+  <si>
+    <t>Nisha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -381,14 +378,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -433,7 +430,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -441,11 +438,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,10 +467,18 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{F8DD23D8-1CC4-498C-AC33-508400D5FC38}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>

</xml_diff>